<commit_message>
30 July 10:00 AM
</commit_message>
<xml_diff>
--- a/testdata/Joy/JOY_Loyalty_Testdata.xlsx
+++ b/testdata/Joy/JOY_Loyalty_Testdata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27923"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86B811C3-3343-417B-A82F-D7554B025F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E24A1ED3-BD58-40CD-9DC1-E54E34F98832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="55" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video_Feedback_AllFdback_Point" sheetId="103" r:id="rId1"/>
@@ -75,42 +75,41 @@
     <sheet name="CompleteChallenge04" sheetId="35" r:id="rId65"/>
     <sheet name="CompleteChallenge03" sheetId="34" r:id="rId66"/>
     <sheet name="CompleteChallenge02" sheetId="33" r:id="rId67"/>
-    <sheet name="CompleteChallenge01.1" sheetId="63" r:id="rId68"/>
-    <sheet name="CompleteChallenge01" sheetId="32" r:id="rId69"/>
-    <sheet name="RaiseContactUsRequest" sheetId="31" r:id="rId70"/>
-    <sheet name="UserDeletion" sheetId="30" r:id="rId71"/>
-    <sheet name="UserCreation" sheetId="29" r:id="rId72"/>
-    <sheet name="UserReactivate" sheetId="28" r:id="rId73"/>
-    <sheet name="GetOKTAUserStatusAfterDeactive" sheetId="27" r:id="rId74"/>
-    <sheet name="UserDeactivate" sheetId="26" r:id="rId75"/>
-    <sheet name="GetOKTAUserStatus" sheetId="25" r:id="rId76"/>
-    <sheet name="GetAccountDetails" sheetId="1" r:id="rId77"/>
-    <sheet name="SpinDetails" sheetId="67" r:id="rId78"/>
-    <sheet name="GetSpin" sheetId="2" r:id="rId79"/>
-    <sheet name="ContactUsInquiry" sheetId="20" r:id="rId80"/>
-    <sheet name="Points" sheetId="8" r:id="rId81"/>
-    <sheet name="Features" sheetId="9" r:id="rId82"/>
-    <sheet name="GetEndingSoon" sheetId="4" r:id="rId83"/>
-    <sheet name="GetExclusiveOrJustIn" sheetId="5" r:id="rId84"/>
-    <sheet name="HotOfferList" sheetId="66" r:id="rId85"/>
-    <sheet name="OffersList" sheetId="17" r:id="rId86"/>
-    <sheet name="MyRewardsList" sheetId="19" r:id="rId87"/>
-    <sheet name="OffersDetails" sheetId="18" r:id="rId88"/>
-    <sheet name="GetBrands" sheetId="22" r:id="rId89"/>
-    <sheet name="Translation" sheetId="6" r:id="rId90"/>
-    <sheet name="Privacy&amp;Policy" sheetId="65" r:id="rId91"/>
-    <sheet name="Terms&amp;Conditions" sheetId="7" r:id="rId92"/>
-    <sheet name="GetFaq" sheetId="21" r:id="rId93"/>
-    <sheet name="Spin_Wedge_Generate" sheetId="23" r:id="rId94"/>
-    <sheet name="GetChallenges" sheetId="3" r:id="rId95"/>
-    <sheet name="CompletedChallenges" sheetId="24" r:id="rId96"/>
-    <sheet name="SurveyList" sheetId="11" r:id="rId97"/>
-    <sheet name="SurveyDetails" sheetId="14" r:id="rId98"/>
-    <sheet name="WallpaperList" sheetId="12" r:id="rId99"/>
-    <sheet name="WallpaperDetails" sheetId="15" r:id="rId100"/>
-    <sheet name="DrawDetail" sheetId="16" r:id="rId101"/>
-    <sheet name="DrawList" sheetId="13" r:id="rId102"/>
-    <sheet name="GetChallengeDetails" sheetId="10" r:id="rId103"/>
+    <sheet name="CompleteChallenge01" sheetId="32" r:id="rId68"/>
+    <sheet name="RaiseContactUsRequest" sheetId="31" r:id="rId69"/>
+    <sheet name="UserDeletion" sheetId="30" r:id="rId70"/>
+    <sheet name="UserCreation" sheetId="29" r:id="rId71"/>
+    <sheet name="UserReactivate" sheetId="28" r:id="rId72"/>
+    <sheet name="GetOKTAUserStatusAfterDeactive" sheetId="27" r:id="rId73"/>
+    <sheet name="UserDeactivate" sheetId="26" r:id="rId74"/>
+    <sheet name="GetOKTAUserStatus" sheetId="25" r:id="rId75"/>
+    <sheet name="GetAccountDetails" sheetId="1" r:id="rId76"/>
+    <sheet name="SpinDetails" sheetId="67" r:id="rId77"/>
+    <sheet name="GetSpin" sheetId="2" r:id="rId78"/>
+    <sheet name="ContactUsInquiry" sheetId="20" r:id="rId79"/>
+    <sheet name="Points" sheetId="8" r:id="rId80"/>
+    <sheet name="Features" sheetId="9" r:id="rId81"/>
+    <sheet name="GetEndingSoon" sheetId="4" r:id="rId82"/>
+    <sheet name="GetExclusiveOrJustIn" sheetId="5" r:id="rId83"/>
+    <sheet name="HotOfferList" sheetId="66" r:id="rId84"/>
+    <sheet name="OffersList" sheetId="17" r:id="rId85"/>
+    <sheet name="MyRewardsList" sheetId="19" r:id="rId86"/>
+    <sheet name="OffersDetails" sheetId="18" r:id="rId87"/>
+    <sheet name="GetBrands" sheetId="22" r:id="rId88"/>
+    <sheet name="Translation" sheetId="6" r:id="rId89"/>
+    <sheet name="Privacy&amp;Policy" sheetId="65" r:id="rId90"/>
+    <sheet name="Terms&amp;Conditions" sheetId="7" r:id="rId91"/>
+    <sheet name="GetFaq" sheetId="21" r:id="rId92"/>
+    <sheet name="Spin_Wedge_Generate" sheetId="23" r:id="rId93"/>
+    <sheet name="GetChallenges" sheetId="3" r:id="rId94"/>
+    <sheet name="CompletedChallenges" sheetId="24" r:id="rId95"/>
+    <sheet name="SurveyList" sheetId="11" r:id="rId96"/>
+    <sheet name="SurveyDetails" sheetId="14" r:id="rId97"/>
+    <sheet name="WallpaperList" sheetId="12" r:id="rId98"/>
+    <sheet name="WallpaperDetails" sheetId="15" r:id="rId99"/>
+    <sheet name="DrawDetail" sheetId="16" r:id="rId100"/>
+    <sheet name="DrawList" sheetId="13" r:id="rId101"/>
+    <sheet name="GetChallengeDetails" sheetId="10" r:id="rId102"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -133,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="111">
   <si>
     <t>Sl#</t>
   </si>
@@ -246,10 +245,10 @@
     <t>true;Reward claimed</t>
   </si>
   <si>
-    <t>success;isPepsicoProduct</t>
+    <t>success;lastInertId</t>
   </si>
   <si>
-    <t>true;true</t>
+    <t>true;NotNull</t>
   </si>
   <si>
     <t>Points added successfully!</t>
@@ -258,7 +257,7 @@
     <t>Duplicate Receipt</t>
   </si>
   <si>
-    <t>true;User deactivated succesfully</t>
+    <t>true;User inactivated succesfully</t>
   </si>
   <si>
     <t>success;type</t>
@@ -292,9 +291,6 @@
   </si>
   <si>
     <t>Challenge already completed!</t>
-  </si>
-  <si>
-    <t>Challenge ID does not exist!</t>
   </si>
   <si>
     <t>Valid-AuthToken-1</t>
@@ -421,12 +417,6 @@
   </si>
   <si>
     <t>title;description;question;answer</t>
-  </si>
-  <si>
-    <t>success;lastInertId</t>
-  </si>
-  <si>
-    <t>true;NotNull</t>
   </si>
   <si>
     <t>title;description;detailDescription;challengeInfoText;challengeEndsInText;termCondition;challengePrimaryText;challengeSecondaryText</t>
@@ -1182,7 +1172,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1373,116 +1363,6 @@
 </file>
 
 <file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C3284D-4869-4084-A2D1-43C77A78ABAD}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="76.5">
-      <c r="A4" s="15">
-        <v>2</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C3C53F-7CDA-4396-8760-13A23E8002E6}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1571,13 +1451,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1591,7 +1471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0849DA21-0394-4189-B9F8-446CA4E2DAC9}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1681,13 +1561,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1701,7 +1581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF10656-5B35-4481-892C-5E1B16F0F457}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1793,13 +1673,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="G4" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3556,8 +3436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4610AE51-8356-4FFC-9989-CCC45CBFCB8B}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4079,7 +3959,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C48914F-6DBE-41FB-93EC-BA440755FA74}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -4138,10 +4020,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4183,7 +4065,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4812,8 +4694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07F64C7-174C-4243-9754-93EF358EFB0B}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5003,7 +4885,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6685,10 +6567,10 @@
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F1DECA-5EB6-4FF6-87CA-629E452A8C2E}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6794,26 +6676,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45.75">
-      <c r="A6" s="22">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -6824,7 +6686,6 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{7EF610AA-ECEF-4169-B8D5-458E0176C07B}"/>
     <hyperlink ref="D5" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{CC11F5D5-23C6-4D4D-8A48-EB25D8770BAA}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{41448BA7-33CD-4FA6-B4EA-6CA124A873E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6832,10 +6693,10 @@
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CD7FBC-0182-4554-A6E5-337AE4356F79}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F6"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6941,26 +6802,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60.75">
-      <c r="A6" s="22">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -6971,7 +6812,6 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{5BEBCC30-F3CD-442D-A952-D7A3FF9F0EFB}"/>
     <hyperlink ref="D5" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{07A8CB40-B9B7-420A-ABEF-AAE7FDD1980C}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{C67CFF80-DE76-4512-A2F5-F5D2EEDC3E72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6979,10 +6819,10 @@
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7EFDF3-674D-4477-858D-0148CC39873C}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" activeCellId="1" sqref="A3:XFD3 A4:XFD4"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7088,26 +6928,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60.75">
-      <c r="A6" s="22">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -7118,7 +6938,6 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{092A65A9-75B8-476A-AAF1-BBD90099B493}"/>
     <hyperlink ref="D5" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{69E087E0-476F-4B71-A3C5-861326ECF00C}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{F72924D6-13E1-4AEA-8175-69B519FF4BEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7126,10 +6945,10 @@
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC68A79-9162-4115-806D-1A1924FE3F09}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F6"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7235,26 +7054,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60.75">
-      <c r="A6" s="22">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -7265,7 +7064,6 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{58C65DFB-035E-4222-B1E7-BB039F615C02}"/>
     <hyperlink ref="D5" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{8584C251-1689-4DB3-9620-EE45DBB9637E}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{BC52AA46-7171-48A1-929D-D2171FC06274}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7439,10 +7237,10 @@
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EBDC33-0B8A-4929-86E3-EE4A80115EF0}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7548,26 +7346,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60.75">
-      <c r="A6" s="22">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -7578,7 +7356,6 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{314E8ADB-D544-4C74-9BD0-9F11D29FFCB3}"/>
     <hyperlink ref="D5" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{C2F8EE89-C302-4D29-A8BF-324864BA3151}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{FE82FACE-0265-4521-BA5C-4DFD7688424E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7586,10 +7363,10 @@
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB86178-A2E3-46AE-B875-57CCD35BD4A3}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7715,26 +7492,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="22">
-        <v>5</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -7746,7 +7503,6 @@
     <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{42CEEAB2-DC44-4E33-ACC9-CED1A4F23EA0}"/>
     <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{4106C97D-6740-40A1-A1DA-8287C9F7E960}"/>
     <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{0C8BA8D4-C170-42AD-AA50-8AE8998543E4}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{2D6D79B4-4B35-4896-9D4C-0DBB4EC51B29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7754,10 +7510,10 @@
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAB067A-CFD9-4F61-858E-77855C7B973D}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7883,26 +7639,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="22">
-        <v>5</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -7914,7 +7650,6 @@
     <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{80115466-81A5-48E6-91E2-F5D2DB4A6514}"/>
     <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{A91727DA-D1E6-4957-A096-E513AAADAABF}"/>
     <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{D7A5EC2E-83EC-422D-A17F-99ACF3F729C1}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{F554148D-9549-499D-B5DD-D6050A5A7ED4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7922,10 +7657,304 @@
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554F8D9E-8340-4C85-A462-2F86902F010B}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{CA90871E-AD3C-405E-89F5-69B36A4C502B}"/>
+    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{D7DE52C8-6B4E-4B0C-94FB-26DBA9B0B530}"/>
+    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{3BC29EF2-C751-4CE5-990E-909D74BA270F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535D8B4D-3FAE-451C-AD3E-90D46CF4682C}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{F30BCDD7-ED98-45E9-AEE7-ACD3A64E5F31}"/>
+    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{23FBE707-2EC4-474A-AB6A-E2C52D413A14}"/>
+    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{C2DB6518-56C7-437F-9F99-0E4F14F84BBC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19304B85-542C-485D-88F1-23DF52D9CC79}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8052,10 +8081,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="22">
-        <v>5</v>
-      </c>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="21">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -8079,27 +8108,27 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{CA90871E-AD3C-405E-89F5-69B36A4C502B}"/>
-    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{D7DE52C8-6B4E-4B0C-94FB-26DBA9B0B530}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{3BC29EF2-C751-4CE5-990E-909D74BA270F}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{0745A692-7038-427C-B86C-E6045B2F2C12}"/>
+    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{FF5B048C-D53F-4FD7-80CF-FEAA52083CB9}"/>
+    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{EC694F39-0489-4C61-B4A4-291D4D7F3E59}"/>
+    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{FEE355D8-799F-4580-BE53-3EA3638910F5}"/>
+    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{72865CB7-C7C4-4B8C-B684-95A51602A3C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535D8B4D-3FAE-451C-AD3E-90D46CF4682C}">
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C3DACA-CB79-4334-B05A-FDDFBC14ECEB}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
@@ -8220,10 +8249,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="22">
-        <v>5</v>
-      </c>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="21">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -8247,21 +8276,315 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{F30BCDD7-ED98-45E9-AEE7-ACD3A64E5F31}"/>
-    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{23FBE707-2EC4-474A-AB6A-E2C52D413A14}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{C2DB6518-56C7-437F-9F99-0E4F14F84BBC}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{04DA79E9-8EE0-416D-A25C-A964B0DA5D18}"/>
+    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{39E40B5C-F681-4080-A1B9-A599B3CA563E}"/>
+    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{CAF34EEB-1A44-4176-A6F9-D6AE24113CE2}"/>
+    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{3972B442-CB34-4DFF-BB17-289C63DEFFB6}"/>
+    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{628FE9E0-8912-48D8-A384-1EA7B93A2410}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19304B85-542C-485D-88F1-23DF52D9CC79}">
-  <dimension ref="A1:F8"/>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB78AB28-3419-404C-9EFA-FD01C43FCB92}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{F6139B90-D4CA-4AB8-80DC-43D8EECA7708}"/>
+    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{F737ABBD-AA57-4F7B-BBE2-989D22762181}"/>
+    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{78FAA298-92D0-426F-9E20-1C9F211ED84F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF507F1A-EEC5-4E33-BDFA-2827B072AC79}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{0318538F-91D4-453B-8F76-A861C08444D2}"/>
+    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{9E7A7969-CDC9-4B2F-8015-4429589ECA97}"/>
+    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{65A9D90E-8A64-446D-A1B1-EDE25AA89BD8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24829EA0-1C43-4105-B09B-4DB178FF1ED8}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8321,110 +8644,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="21">
-        <v>5</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30.75">
-      <c r="A8" s="19">
-        <v>6</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -8435,642 +8658,7 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{FF5B048C-D53F-4FD7-80CF-FEAA52083CB9}"/>
-    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{EC694F39-0489-4C61-B4A4-291D4D7F3E59}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{FEE355D8-799F-4580-BE53-3EA3638910F5}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{72865CB7-C7C4-4B8C-B684-95A51602A3C5}"/>
-    <hyperlink ref="D8" r:id="rId5" display="vajralaskr1994@gmail.com" xr:uid="{D01FDC32-81FD-40B4-A248-8EFB484F2820}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C3DACA-CB79-4334-B05A-FDDFBC14ECEB}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="21">
-        <v>5</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30.75">
-      <c r="A8" s="19">
-        <v>6</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{39E40B5C-F681-4080-A1B9-A599B3CA563E}"/>
-    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{CAF34EEB-1A44-4176-A6F9-D6AE24113CE2}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{3972B442-CB34-4DFF-BB17-289C63DEFFB6}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{628FE9E0-8912-48D8-A384-1EA7B93A2410}"/>
-    <hyperlink ref="D8" r:id="rId5" display="vajralaskr1994@gmail.com" xr:uid="{6F59E149-E3B0-444C-874E-E5C758DC249F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB78AB28-3419-404C-9EFA-FD01C43FCB92}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60.75">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{F6139B90-D4CA-4AB8-80DC-43D8EECA7708}"/>
-    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{F737ABBD-AA57-4F7B-BBE2-989D22762181}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{78FAA298-92D0-426F-9E20-1C9F211ED84F}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{A9595264-EE82-4510-BD38-A6873899B5B2}"/>
-    <hyperlink ref="D8" r:id="rId5" display="vajralaskr1994@gmail.com" xr:uid="{05ADC599-0CB8-4E5A-8530-7AF3148649D2}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B0DC03-4227-4F96-9E84-5BD62BDE13DA}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{B9DAA3B3-AFCC-47E6-A109-4663F0DC7686}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF507F1A-EEC5-4E33-BDFA-2827B072AC79}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60.75">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{0318538F-91D4-453B-8F76-A861C08444D2}"/>
-    <hyperlink ref="D4" r:id="rId2" display="vajralaskr1994@gmail.com" xr:uid="{9E7A7969-CDC9-4B2F-8015-4429589ECA97}"/>
-    <hyperlink ref="D6" r:id="rId3" display="vajralaskr1994@gmail.com" xr:uid="{65A9D90E-8A64-446D-A1B1-EDE25AA89BD8}"/>
-    <hyperlink ref="D7" r:id="rId4" display="vajralaskr1994@gmail.com" xr:uid="{DB514237-EF99-4E45-8734-B4E67BD3F411}"/>
+    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{20922494-387B-419D-B2E7-336478E95909}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9245,91 +8833,6 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24829EA0-1C43-4105-B09B-4DB178FF1ED8}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="vajralaskr1994@gmail.com" xr:uid="{20922494-387B-419D-B2E7-336478E95909}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD289CC-9039-4F0F-BC86-D22600AE2E3E}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -9385,19 +8888,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -9405,19 +8908,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9425,19 +8928,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -9456,7 +8959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAB51D3-77AA-44F1-8EEE-D5582915DC5D}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -9512,19 +9015,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -9532,19 +9035,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9552,19 +9055,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -9583,7 +9086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B12004-62EA-4E88-A5D5-FE71E814E7A5}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -9639,19 +9142,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -9659,19 +9162,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9679,19 +9182,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -9710,7 +9213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F690F3F-5B7B-4074-A36D-47763A924E42}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -9766,19 +9269,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -9786,19 +9289,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9806,19 +9309,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -9837,7 +9340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD08A7F-4F66-40B0-A02D-2EBF64451B55}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -9893,16 +9396,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
@@ -9913,19 +9416,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9933,19 +9436,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -9964,7 +9467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5103DD93-3C3A-4079-A31B-A8EFE9C77215}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -10020,16 +9523,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
@@ -10040,19 +9543,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -10060,19 +9563,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -10091,7 +9594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -10176,7 +9679,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>
@@ -10196,7 +9699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41551EB8-C819-4BDA-A4A3-38F3A7C38BD4}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -10289,13 +9792,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -10309,7 +9812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B85C9A9-D503-4586-906B-A86D3043DCB9}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -10402,13 +9905,99 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="4" t="s">
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BB3897-6005-4203-9500-CFB03F783710}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30.75">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>69</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -10591,92 +10180,6 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BB3897-6005-4203-9500-CFB03F783710}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30.75">
-      <c r="A3" s="15">
-        <v>2</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F93423-B7C1-4C7E-B541-6003B7B81E00}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -10739,7 +10242,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
@@ -10759,7 +10262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE1148F-8963-452A-8419-B6B318435697}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -10815,19 +10318,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -10841,7 +10344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16037CF-55CA-4E5C-8162-2720EDED988D}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -10934,13 +10437,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -10954,7 +10457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122BC05C-234E-409D-96A6-075E6E6F1FAB}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -11047,13 +10550,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -11067,7 +10570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF4040-4C56-4F17-80FC-6DF26852CE70}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -11156,13 +10659,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -11176,7 +10679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5DC4F1-ACAD-44CF-AA9B-DA14D83A3175}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -11267,13 +10770,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -11287,12 +10790,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0429301-5852-4D35-A263-58CBB557DFDB}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11376,13 +10879,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="G4" s="16" t="s">
         <v>83</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -11396,7 +10899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB222E47-BCB4-4C8C-9762-591DA7129F99}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -11486,13 +10989,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -11506,7 +11009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7635F4A0-2416-4EA6-92B4-7C14A325AE66}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -11596,13 +11099,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -11611,6 +11114,85 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6650D58-1081-4CB5-ADC1-3B8AD1D4418D}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="50"/>
+      <c r="E1" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="50"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11707,85 +11289,6 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6650D58-1081-4CB5-ADC1-3B8AD1D4418D}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E1245C-FA77-49ED-A04A-E6A6EC3A3821}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -11842,22 +11345,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -11871,7 +11374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A358A6-B854-4A98-BB65-8A9762765299}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -11928,22 +11431,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -11957,7 +11460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5872E88F-138F-438C-83CD-91DBA8CFA546}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -11979,7 +11482,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>1</v>
@@ -12018,7 +11521,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -12027,13 +11530,13 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -12047,7 +11550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D22535-5CAC-4DC2-A409-549988810C74}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -12132,10 +11635,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -12152,7 +11655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C3B886-15D0-4923-92A9-1F481A2C02E8}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -12245,13 +11748,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -12265,7 +11768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8975BC-A7E7-4248-B90B-ED2ADBEE4B3F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -12354,13 +11857,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="G4" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -12374,7 +11877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBCF62F-DF35-4C67-9759-09D627C9559D}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -12467,10 +11970,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>26</v>
@@ -12487,7 +11990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA575631-A1A8-491C-94B9-235B6FD95CC8}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -12578,10 +12081,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>26</v>
@@ -12592,19 +12095,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>11</v>
@@ -12615,19 +12118,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>11</v>
@@ -12644,7 +12147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8810-F278-4E99-BBDE-40FE212A77E1}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -12733,10 +12236,120 @@
         <v>5</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C3284D-4869-4084-A2D1-43C77A78ABAD}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="76.5">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
01 Aug 10:00 AM
</commit_message>
<xml_diff>
--- a/testdata/Joy/JOY_Loyalty_Testdata.xlsx
+++ b/testdata/Joy/JOY_Loyalty_Testdata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27923"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27927"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E24A1ED3-BD58-40CD-9DC1-E54E34F98832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F8E839-7925-459E-9EE9-50A6E3B43218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="55" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="28" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video_Feedback_AllFdback_Point" sheetId="103" r:id="rId1"/>
@@ -3960,7 +3960,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4020,7 +4020,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>

</xml_diff>